<commit_message>
Updated Project plan Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moamen\Desktop\SWE\SW deliveries log\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10BFBB6-0BBE-4413-9739-6A0B4A303483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>Team member</t>
   </si>
@@ -117,9 +126,6 @@
   </si>
   <si>
     <t>Update SRS Document</t>
-  </si>
-  <si>
-    <t>3 days</t>
   </si>
   <si>
     <t>update the formating of the SRS document and modify it to match the updated CYRS document</t>
@@ -137,28 +143,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -168,7 +175,13 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -182,75 +195,69 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -440,32 +447,37 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.0"/>
-    <col customWidth="1" min="2" max="2" width="35.43"/>
-    <col customWidth="1" min="3" max="3" width="17.86"/>
-    <col customWidth="1" min="4" max="4" width="16.14"/>
-    <col customWidth="1" min="5" max="5" width="20.57"/>
-    <col customWidth="1" min="6" max="6" width="18.14"/>
-    <col customWidth="1" min="7" max="7" width="43.0"/>
-    <col customWidth="1" min="8" max="8" width="18.71"/>
-    <col customWidth="1" min="9" max="9" width="20.57"/>
-    <col customWidth="1" min="10" max="10" width="18.71"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="43" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -523,7 +535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -549,7 +561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -575,7 +587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="20.25" customHeight="1">
+    <row r="5" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -601,7 +613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" ht="30.0" customHeight="1">
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -612,10 +624,10 @@
         <v>27</v>
       </c>
       <c r="D6" s="5">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="E6" s="5">
-        <v>43865.0</v>
+        <v>43866</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>28</v>
@@ -629,7 +641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -640,10 +652,10 @@
         <v>27</v>
       </c>
       <c r="D7" s="5">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="E7" s="5">
-        <v>43865.0</v>
+        <v>43866</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>28</v>
@@ -657,7 +669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" ht="39.0" customHeight="1">
+    <row r="8" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -668,16 +680,16 @@
         <v>27</v>
       </c>
       <c r="D8" s="5">
-        <v>43865.0</v>
+        <v>43866</v>
       </c>
       <c r="E8" s="5">
-        <v>43868.0</v>
+        <v>43868</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
@@ -685,33 +697,35 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="5">
-        <v>43868.0</v>
+        <v>43868</v>
       </c>
       <c r="E9" s="5">
-        <v>43868.0</v>
+        <v>43868</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10">
+      <c r="J9" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -723,7 +737,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -735,7 +749,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -747,7 +761,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -759,7 +773,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -771,7 +785,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -783,7 +797,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -795,7 +809,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -807,7 +821,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -819,7 +833,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -831,7 +845,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -843,7 +857,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -855,7 +869,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -867,7 +881,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -879,7 +893,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -891,7 +905,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -903,7 +917,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -915,7 +929,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -927,7 +941,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -939,7 +953,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -951,7 +965,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -963,7 +977,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -975,7 +989,7 @@
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -987,7 +1001,7 @@
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -999,7 +1013,7 @@
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -1011,7 +1025,7 @@
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -1024,20 +1038,21 @@
       <c r="J35" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Project Plan with a minor task to edit the SRS document Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moamen\Desktop\SWE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4B49B2-6D75-4E61-985D-C3259B2BF0B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F68AFD8-B21C-4CDA-8F4E-DC8ABE58C9AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Team member</t>
   </si>
@@ -171,6 +171,21 @@
   </si>
   <si>
     <t>Review SRS document and make sure it follows the review document and guidlines</t>
+  </si>
+  <si>
+    <t>Mina Yousry</t>
+  </si>
+  <si>
+    <t>Minor updates to SRS document</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>Remove document status and add status table</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -580,7 +595,7 @@
   <dimension ref="A1:J1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -982,14 +997,30 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="27"/>
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="6">
+        <v>43869</v>
+      </c>
+      <c r="E15" s="6">
+        <v>43869</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="5"/>
     </row>

</xml_diff>

<commit_message>
Reviewed and added comments on SRS document to project plan Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Team member</t>
   </si>
@@ -175,20 +175,33 @@
     <t>Remove document status and add status table</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>3 days</t>
   </si>
   <si>
     <t>Update the SRS document according the presentation provided and the SRS review sheet</t>
+  </si>
+  <si>
+    <t>Split Req_PO1_DGC_SRS_002_v1.1 and Req_PO1_DGC_SRS_003_v1.1 tables
+Add SRS context diagram
+Add testing scope ITD or VTD
+Req_PO1_DGC_SRS_003_v1.1
+Req_PO1_DGC_SRS_006_v1.1
+Req_PO1_DGC_SRS_009_v1.1
+Req_PO1_DGC_SRS_0013_v1.1
+Clarify the shall display which data on the LCD
+Req_PO1_DGC_SRS_0019_v1.1
+Remove variable write number instead
+Req_PO1_DGC_SRS_0020_v1.1
+remove cast write display instead
+Req_PO1_DGC_SRS_0023_v1.1
+time is 15 seconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -197,10 +210,6 @@
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -302,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -347,18 +356,14 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,7 +594,7 @@
     <col customWidth="1" min="6" max="6" width="18.14"/>
     <col customWidth="1" min="7" max="7" width="43.0"/>
     <col customWidth="1" min="8" max="8" width="18.71"/>
-    <col customWidth="1" min="9" max="9" width="35.29"/>
+    <col customWidth="1" min="9" max="9" width="57.71"/>
     <col customWidth="1" hidden="1" min="10" max="10" width="14.43"/>
   </cols>
   <sheetData>
@@ -999,38 +1004,40 @@
       <c r="G15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>53</v>
+      <c r="H15" s="22" t="s">
+        <v>15</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" ht="27.0" customHeight="1">
-      <c r="A16" s="22" t="s">
+    <row r="16" ht="259.5" customHeight="1">
+      <c r="A16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>43879.0</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="23">
         <v>43881.0</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="H16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="3"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Assigned a task to modify SRS document according to review Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>Team member</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Remove document status and add status table</t>
-  </si>
-  <si>
-    <t>3 days</t>
   </si>
   <si>
     <t>Update the SRS document according the presentation provided and the SRS review sheet</t>
@@ -196,12 +193,18 @@
 Req_PO1_DGC_SRS_0023_v1.1
 time is 15 seconds</t>
   </si>
+  <si>
+    <t>Update SRS document according to previous review</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -210,6 +213,10 @@
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -311,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -363,7 +370,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1026,29 +1043,45 @@
       <c r="E16" s="23">
         <v>43881.0</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>54</v>
       </c>
       <c r="H16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" ht="27.75" customHeight="1">
+      <c r="A17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="27">
+        <v>43880.0</v>
+      </c>
+      <c r="E17" s="23">
+        <v>43881.0</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="J17" s="5"/>
     </row>

</xml_diff>

<commit_message>
Updated project plan with new task Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
   <si>
     <t>Team member</t>
   </si>
@@ -197,7 +197,25 @@
     <t>Update SRS document according to previous review</t>
   </si>
   <si>
+    <t>Update SRS document according to SRS review sheet</t>
+  </si>
+  <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Create GDD document and layered architecture</t>
+  </si>
+  <si>
+    <t>Initial creation of GDD document and initial layered architecture</t>
+  </si>
+  <si>
+    <t>Create APIs for the Application layer</t>
+  </si>
+  <si>
+    <t>Create APIs for the HAL layer</t>
+  </si>
+  <si>
+    <t>Create APIs for the MCAL layer</t>
   </si>
 </sst>
 </file>
@@ -318,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -363,17 +381,18 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -609,7 +628,7 @@
     <col customWidth="1" min="4" max="4" width="16.14"/>
     <col customWidth="1" min="5" max="5" width="20.57"/>
     <col customWidth="1" min="6" max="6" width="18.14"/>
-    <col customWidth="1" min="7" max="7" width="43.0"/>
+    <col customWidth="1" min="7" max="7" width="46.57"/>
     <col customWidth="1" min="8" max="8" width="18.71"/>
     <col customWidth="1" min="9" max="9" width="57.71"/>
     <col customWidth="1" hidden="1" min="10" max="10" width="14.43"/>
@@ -1043,7 +1062,7 @@
       <c r="E16" s="23">
         <v>43881.0</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="17" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="18" t="s">
@@ -1052,96 +1071,170 @@
       <c r="H16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="24" t="s">
         <v>54</v>
       </c>
       <c r="J16" s="5"/>
     </row>
     <row r="17" ht="27.75" customHeight="1">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="23">
         <v>43880.0</v>
       </c>
       <c r="E17" s="23">
         <v>43881.0</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="22" t="s">
-        <v>56</v>
+      <c r="H17" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
+      <c r="A18" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="28">
+        <v>43886.0</v>
+      </c>
+      <c r="E18" s="28">
+        <v>43887.0</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="I18" s="3"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="4"/>
+    <row r="19" ht="33.0" customHeight="1">
+      <c r="A19" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="28">
+        <v>43886.0</v>
+      </c>
+      <c r="E19" s="28">
+        <v>43888.0</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="5"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="A20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="28">
+        <v>43886.0</v>
+      </c>
+      <c r="E20" s="28">
+        <v>43888.0</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="28">
+        <v>43886.0</v>
+      </c>
+      <c r="E21" s="28">
+        <v>43888.0</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="J21" s="5"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="A22" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="28">
+        <v>43886.0</v>
+      </c>
+      <c r="E22" s="28">
+        <v>43888.0</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="J22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Updated RTM and project plan Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project Plan.xlsx
+++ b/SW deliveries log/Project Plan.xlsx
@@ -224,10 +224,10 @@
     <t>Update RTM with GDD requirements</t>
   </si>
   <si>
+    <t>Create CDD for Buzzer</t>
+  </si>
+  <si>
     <t>Pending</t>
-  </si>
-  <si>
-    <t>Create CDD for Buzzer</t>
   </si>
   <si>
     <t>Create CDD for DIO</t>
@@ -1354,8 +1354,8 @@
         <v>14</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="22" t="s">
-        <v>65</v>
+      <c r="H26" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="5"/>
@@ -1365,7 +1365,7 @@
         <v>16</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>26</v>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="5"/>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="5"/>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="5"/>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="5"/>

</xml_diff>